<commit_message>
design, task fixed, time therapy duration...
</commit_message>
<xml_diff>
--- a/Templates/User_template.xlsx
+++ b/Templates/User_template.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Aleksandar\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Koja_project\custom_management\Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="19">
   <si>
     <t>email</t>
   </si>
@@ -61,9 +61,6 @@
   </si>
   <si>
     <t>storeId</t>
-  </si>
-  <si>
-    <t>img</t>
   </si>
   <si>
     <t>test</t>
@@ -84,7 +81,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -444,11 +441,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P2"/>
+  <dimension ref="A1:O2"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="N2" sqref="N2"/>
+      <selection pane="bottomLeft" activeCell="P6" sqref="P6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -459,9 +456,9 @@
     <col min="6" max="6" width="17" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>5</v>
@@ -505,46 +502,43 @@
       <c r="O1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="P1" s="1" t="s">
-        <v>14</v>
-      </c>
     </row>
-    <row r="2" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>16</v>
-      </c>
       <c r="D2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J2">
         <v>112</v>
       </c>
       <c r="K2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="L2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="M2">
         <v>3</v>
@@ -554,9 +548,6 @@
       </c>
       <c r="O2">
         <v>0</v>
-      </c>
-      <c r="P2" t="s">
-        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>